<commit_message>
Carte Match à Mort
Version du jeu permettant de tester la carte Match à Mort
</commit_message>
<xml_diff>
--- a/APK_SpaceBattle/liste versions.xlsx
+++ b/APK_SpaceBattle/liste versions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B65DA24-1462-4620-823B-1099F2A36D38}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417A4D81-1B4D-4AE2-9B09-B9D4BA75870B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>Ajout des tirs (+ collisions des tirs</t>
+  </si>
+  <si>
+    <t>0.5.1</t>
+  </si>
+  <si>
+    <t>Correctif tirs et bouton tir</t>
+  </si>
+  <si>
+    <t>0.5.2</t>
+  </si>
+  <si>
+    <t>Correctif tirs (probleme de mort réguliere) + ajout icone</t>
+  </si>
+  <si>
+    <t>0.5.3</t>
+  </si>
+  <si>
+    <t>Correctif tirs (cadence+morts) + modif icone</t>
   </si>
 </sst>
 </file>
@@ -383,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,6 +490,39 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43397</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43398</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43398</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>